<commit_message>
Update documentation website content
</commit_message>
<xml_diff>
--- a/docs/resources/doc_tables.xlsx
+++ b/docs/resources/doc_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czippel\Documents\GitHub\sandbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czippel\Documents\GitHub\getcensus\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE15D18-6CF2-43EC-9018-2424E117944D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBABDC8-1CD6-4B51-9119-1F7CE65E54AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="15930" windowHeight="9240" xr2:uid="{614A9CB4-755C-45CD-BCD3-7F2BDDFCA0D2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{614A9CB4-755C-45CD-BCD3-7F2BDDFCA0D2}"/>
   </bookViews>
   <sheets>
     <sheet name="geographies" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>Detailed renter housing cost burden*</t>
+  </si>
+  <si>
+    <t>statefips&lt;sup&gt;‡&lt;/sup&gt;</t>
   </si>
 </sst>
 </file>
@@ -735,13 +738,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F240D3E0-4FF9-4926-B14C-70DCEF4D2853}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -752,22 +755,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -775,7 +778,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -786,7 +789,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -800,7 +803,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -811,7 +814,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -825,7 +828,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -833,7 +836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -844,10 +847,10 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -861,7 +864,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -875,7 +878,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -886,7 +889,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -897,7 +900,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -908,7 +911,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -919,7 +922,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -930,7 +933,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -941,7 +944,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -949,7 +952,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -963,7 +966,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -971,7 +974,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -979,7 +982,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -987,7 +990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>26</v>
       </c>
@@ -1005,18 +1008,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC423CC-ED26-4BD0-88E5-4652E112A278}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="1"/>
-    <col min="2" max="2" width="43.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="43.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43</v>
       </c>
@@ -1186,17 +1189,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DD25C4-A271-4D4C-8519-DA5D6FC2E821}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>99</v>
       </c>

</xml_diff>